<commit_message>
edits of file excel
</commit_message>
<xml_diff>
--- a/public/files/Pinger_Excel_Template.xlsx
+++ b/public/files/Pinger_Excel_Template.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>name</t>
   </si>
@@ -212,10 +212,13 @@
     <t>switch_model_id</t>
   </si>
   <si>
-    <t>entuity_status</t>
-  </si>
-  <si>
-    <t>Entuty_add-id</t>
+    <t>entuty_status_id</t>
+  </si>
+  <si>
+    <t>added_on_entuity</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,10 +668,10 @@
         <v>24</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="AA1" t="s">
         <v>25</v>
@@ -792,8 +795,8 @@
       <c r="X2" t="s">
         <v>49</v>
       </c>
-      <c r="Y2">
-        <v>1</v>
+      <c r="Y2" t="s">
+        <v>62</v>
       </c>
       <c r="Z2" t="s">
         <v>51</v>

</xml_diff>